<commit_message>
montagem de banco de dados
</commit_message>
<xml_diff>
--- a/empenhar.xlsx
+++ b/empenhar.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Nº BM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P/G</t>
+  </si>
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -46,6 +52,12 @@
     <t xml:space="preserve">DOC SEI</t>
   </si>
   <si>
+    <t xml:space="preserve">142.998-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Ten</t>
+  </si>
+  <si>
     <t xml:space="preserve">José Carlos</t>
   </si>
   <si>
@@ -58,6 +70,12 @@
     <t xml:space="preserve">1400.01.0051032/2024-02</t>
   </si>
   <si>
+    <t xml:space="preserve">142.998-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Ten</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maria Josefina</t>
   </si>
   <si>
@@ -65,6 +83,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 1400.01.0057532/2024-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142.998-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Sgt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142.998-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cb</t>
   </si>
 </sst>
 </file>
@@ -117,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -125,6 +155,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -151,17 +188,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -185,16 +234,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -204,13 +255,13 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -219,116 +270,146 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="n">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>12345678987</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>1234</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="H2" s="4" t="n">
         <v>753159</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="I2" s="4" t="n">
         <v>123456789</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>98765421</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>3578</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>567899</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>456789878</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>98765421</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>3578</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>567899</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>456789878</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="E4" s="4" t="n">
+        <v>12345678987</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="G4" s="4" t="n">
+        <v>1234</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>753159</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="n">
         <v>12345678987</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="n">
         <v>1234</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="H5" s="4" t="n">
         <v>753159</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="I5" s="4" t="n">
         <v>123456789</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>12345678987</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1234</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>753159</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>11</v>
+      <c r="J5" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3"/>
+      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>